<commit_message>
Update PPDM Cookies Category TestCases Prathima.xlsx
Updated TC Cookie Categories
</commit_message>
<xml_diff>
--- a/PPDM Cookies Category TestCases Prathima.xlsx
+++ b/PPDM Cookies Category TestCases Prathima.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b74f996c24ffab3a/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{78264F3F-F76F-4952-BD6A-715F5A219400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DC0B52C-60B1-4366-BF91-EB11C7803433}"/>
+  <xr:revisionPtr revIDLastSave="213" documentId="8_{78264F3F-F76F-4952-BD6A-715F5A219400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F711A1DA-9A2E-493B-8C94-6223736DC556}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{DD5ADD8E-8C9E-4FCC-80B5-415D51444A41}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{DD5ADD8E-8C9E-4FCC-80B5-415D51444A41}"/>
   </bookViews>
   <sheets>
     <sheet name="Analyticcookies Gov" sheetId="1" r:id="rId1"/>
     <sheet name="Adobe Analyticcookies" sheetId="2" r:id="rId2"/>
+    <sheet name="StrictlyNecessarycookies" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="171">
   <si>
     <t>Test Scenario ID</t>
   </si>
@@ -192,10 +193,364 @@
     <t>TC_AAC_8</t>
   </si>
   <si>
-    <t>TC_AAC_9</t>
-  </si>
-  <si>
-    <t>TC_AAC_10</t>
+    <t>Adobe Analytical cookie name s_cc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Adobe Analytical cookie name  s_cc  and its purpose and expires .</t>
+  </si>
+  <si>
+    <t>Analytical cookie Name s_cc</t>
+  </si>
+  <si>
+    <t>Analytical cookie s_cc appears</t>
+  </si>
+  <si>
+    <t>1.open the link https://www.nhs.uk/our-policies/cookies-policy/ 2.Move down to analytical cookie s_cc .</t>
+  </si>
+  <si>
+    <t>Analytical cookie s_cc appears and its purpose and expires time are seen</t>
+  </si>
+  <si>
+    <t>Analytical cookie s_cc should appear and its purpose and expire time should be seen</t>
+  </si>
+  <si>
+    <t>Adobe Analytical cookie name s_sq</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Adobe Analytical cookie name  s_sq and its purpose and expires .</t>
+  </si>
+  <si>
+    <t>Analytical cookie Name s_sq</t>
+  </si>
+  <si>
+    <t>Analytical cookie s_sq appears</t>
+  </si>
+  <si>
+    <t>1.open the link https://www.nhs.uk/our-policies/cookies-policy/ 2.Move down to analytical cookie s_sq .</t>
+  </si>
+  <si>
+    <t>Analytical cookie s_sq appears and its purpose and expires time are seen</t>
+  </si>
+  <si>
+    <t>Analytical cookie s_sq should appear and its purpose and expire time should be seen</t>
+  </si>
+  <si>
+    <t>Adobe Analytical cookie name AMCV_###@AdobeOrg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Adobe Analytical cookie name  AMCV_###@AdobeOrg  and its purpose and expires .</t>
+  </si>
+  <si>
+    <t>Analytical cookie Name AMCV_###@AdobeOrg</t>
+  </si>
+  <si>
+    <t>Analytical cookie AMCV_###@AdobeOrg appears</t>
+  </si>
+  <si>
+    <t>1.open the link https://www.nhs.uk/our-policies/cookies-policy/ 2.Move down to analytical cookie AMCV_###@AdobeOrg .</t>
+  </si>
+  <si>
+    <t>Analytical cookie AMCV_###@AdobeOrg appears and its purpose and expires time are seen</t>
+  </si>
+  <si>
+    <t>Analytical cookie AMCV_###@AdobeOrg should appear and its purpose and expire time should be seen</t>
+  </si>
+  <si>
+    <t>Adobe Analytical cookie name AMCVS_###@AdobeOrg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Adobe Analytical cookie name  AMCVS_###@AdobeOrg  and its purpose and expires .</t>
+  </si>
+  <si>
+    <t>Analytical cookie Name AMCVS_###@AdobeOrg</t>
+  </si>
+  <si>
+    <t>Analytical cookie AMCVS_###@AdobeOrg appears</t>
+  </si>
+  <si>
+    <t>1.open the link https://www.nhs.uk/our-policies/cookies-policy/ 2.Move down to analytical cookie AMCVS_###@AdobeOrg.</t>
+  </si>
+  <si>
+    <t>Analytical cookie AMCVS_###@AdobeOrg appears and its purpose and expires time are seen</t>
+  </si>
+  <si>
+    <t>Analytical cookie AMCVS_###@AdobeOrg should appear and its purpose and expire time should be seen</t>
+  </si>
+  <si>
+    <t>Adobe Analytical cookie name Gpv</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Adobe Analytical cookie name  Gpv and its purpose and expires .</t>
+  </si>
+  <si>
+    <t>Analytical cookie Name Gpv</t>
+  </si>
+  <si>
+    <t>Analytical cookie Gpv appears</t>
+  </si>
+  <si>
+    <t>1.open the link https://www.nhs.uk/our-policies/cookies-policy/ 2.Move down to analytical cookie Gpv .</t>
+  </si>
+  <si>
+    <t>Analytical cookie Gpv appears and its purpose and expires time are seen</t>
+  </si>
+  <si>
+    <t>Analytical cookie Gpv should appear and its purpose and expire time should be seen</t>
+  </si>
+  <si>
+    <t>Adobe Analytical cookie name s_ppv</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Adobe Analytical cookie name  s_ppv  and its purpose and expires .</t>
+  </si>
+  <si>
+    <t>Analytical cookie Name s_ppv</t>
+  </si>
+  <si>
+    <t>Analytical cookie s_ppv appears</t>
+  </si>
+  <si>
+    <t>1.open the link https://www.nhs.uk/our-policies/cookies-policy/ 2.Move down to analytical cookie s_ppv .</t>
+  </si>
+  <si>
+    <t>Analytical cookie s_ppv appears and its purpose and expires time are seen</t>
+  </si>
+  <si>
+    <t>Analytical cookie s_ppv should appear and its purpose and expire time should be seen</t>
+  </si>
+  <si>
+    <t>Adobe Analytical cookie name s_tp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Adobe Analytical cookie name  s_tp  and its purpose and expires .</t>
+  </si>
+  <si>
+    <t>Analytical cookie Name s_tp</t>
+  </si>
+  <si>
+    <t>Analytical cookie s_tp appears</t>
+  </si>
+  <si>
+    <t>1.open the link https://www.nhs.uk/our-policies/cookies-policy/ 2.Move down to analytical cookie s_tp .</t>
+  </si>
+  <si>
+    <t>Analytical cookie s_tp appears and its purpose and expires time are seen</t>
+  </si>
+  <si>
+    <t>Analytical cookie  s_tp should appear and its purpose and expire time should be seen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cookie name HideBiometricBanner</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie name  HideBiometricBanner and its purpose and expires .</t>
+  </si>
+  <si>
+    <t>TC_SNC_1</t>
+  </si>
+  <si>
+    <t>TC_SNC_2</t>
+  </si>
+  <si>
+    <t>TC_SNC_3</t>
+  </si>
+  <si>
+    <t>TC_SNC_4</t>
+  </si>
+  <si>
+    <t>TC_SNC_5</t>
+  </si>
+  <si>
+    <t>TC_SNC_6</t>
+  </si>
+  <si>
+    <t>TC_SNC_7</t>
+  </si>
+  <si>
+    <t>TC_SNC_8</t>
+  </si>
+  <si>
+    <t>Adobe Analytical cookie name s_getNewRepeat</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Adobe Analytical cookie name  s_getNewRepeat  and its purpose and expires .</t>
+  </si>
+  <si>
+    <t>Analytical cookie Name s_getNewRepeat</t>
+  </si>
+  <si>
+    <t>Analytical cookie s_getNewRepeat appears</t>
+  </si>
+  <si>
+    <t>1.open the link https://www.nhs.uk/our-policies/cookies-policy/ 2.Move down to analytical cookie s_getNewRepeat .</t>
+  </si>
+  <si>
+    <t>Analytical cookie s_getNewRepeat appears and its purpose and expires time are seen</t>
+  </si>
+  <si>
+    <t>Analytical cookie  s_getNewRepeat should appear and its purpose and expire time should be seen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cookie name nhso.session</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie name  nhso.session and its purpose and expires .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strictly necessary cookie Name HideBiometricBanner </t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie HideBiometricBanner  appears</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie HideBiometricBanner  appears and its purpose and expires time are seen</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie HideBiometricBanner  should appear and its purpose and expire time should be seen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strictly necessary cookie Name nhso.session </t>
+  </si>
+  <si>
+    <t>1.open the link https://www.nhs.uk/our-policies/cookies-policy/ 2.Move down to Strictly necessary cookie HideBiometricBanner  .</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie nhso.session  appears</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie  nhso.session  appears and its purpose and expires time are seen</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie  nhso.session should appear and its purpose and expire time should be seen</t>
+  </si>
+  <si>
+    <t>1.open the link https://www.nhs.uk/our-policies/cookies-policy/ 2.Move down to Strictly necessary cookie  nhso.session  .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cookie name NHSO-Session-Id</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie name  NHSO-Session-Id and its purpose and expires .</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie Name NHSO-Session-Id</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie NHSO-Session-Id  appears</t>
+  </si>
+  <si>
+    <t>1.open the link https://www.nhs.uk/our-policies/cookies-policy/ 2.Move down to Strictly necessary cookie  NHSO-Session-Id  .</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie  NHSO-Session-Id  appears and its purpose and expires time are seen</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie  NHSO-Session-Id should appear and its purpose and expire time should be seen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cookie name nhso.authr</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie name  nhso.auth and its purpose and expires .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strictly necessary cookie Name nhso.auth </t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie nhso.auth  appears</t>
+  </si>
+  <si>
+    <t>1.open the link https://www.nhs.uk/our-policies/cookies-policy/ 2.Move down to Strictly necessary cookie  nhso.auth  .</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie  nhso.auth  appears and its purpose and expires time are seen</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie  nhso.auth should appear and its purpose and expire time should be seen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cookie name nhso.terms</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie name  nhso.terms and its purpose and expires .</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie Name nhso.terms</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie nhso.terms  appears</t>
+  </si>
+  <si>
+    <t>1.open the link https://www.nhs.uk/our-policies/cookies-policy/ 2.Move down to Strictly necessary cookie  nhso.terms  .</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie  nhso.terms  appears and its purpose and expires time are seen</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie  nhso.terms should appear and its purpose and expire time should be seen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cookie name nhso.notifications-prompt-###</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cookie name NHSO-Session-Expiry</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie name  NHSO-Session-Expiry and its purpose and expires .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strictly necessary cookie Name NHSO-Session-Expiry </t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie NHSO-Session-Expiry  appears</t>
+  </si>
+  <si>
+    <t>1.open the link https://www.nhs.uk/our-policies/cookies-policy/ 2.Move down to Strictly necessary cookie  NHSO-Session-Expiry  .</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie  NHSO-Session-Expiry  appears and its purpose and expires time are seen</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie  NHSO-Session-Expiry should appear and its purpose and expire time should be seen</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie name  nhso.notifications-prompt-### and its purpose and expires .</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie Name nhso.notifications-prompt-###</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie nhso.notifications-prompt-###  appears</t>
+  </si>
+  <si>
+    <t>1.open the link https://www.nhs.uk/our-policies/cookies-policy/ 2.Move down to Strictly necessary cookie  nhso.notifications-prompt-###  .</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie  nhso.notifications-prompt-###  appears and its purpose and expires time are seen</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie  nhso.notifications-prompt-### should appear and its purpose and expire time should be seen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cookie name SkipPreRegistrationPage</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie name  SkipPreRegistrationPage and its purpose and expires .</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie Name SkipPreRegistrationPage</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie SkipPreRegistrationPage appears</t>
+  </si>
+  <si>
+    <t>1.open the link https://www.nhs.uk/our-policies/cookies-policy/ 2.Move down to Strictly necessary cookie SkipPreRegistrationPage.</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie  SkipPreRegistrationPage appears and its purpose and expires time are seen</t>
+  </si>
+  <si>
+    <t>Strictly necessary cookie  SkipPreRegistrationPage should appear and its purpose and expire time should be seen</t>
   </si>
 </sst>
 </file>
@@ -609,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5647211A-0140-4C56-8B72-7A15036C5DD1}">
   <dimension ref="B3:L42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1247,10 +1602,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DC6BFC0-268A-4180-96A7-345D3D15841B}">
-  <dimension ref="B3:L13"/>
+  <dimension ref="B3:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:K12"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1300,139 +1655,591 @@
       </c>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:12" ht="116" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="C4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:12" ht="116" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="C5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:12" ht="145" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="C6" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>78</v>
+      </c>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:12" ht="145" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="C7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:12" ht="116" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+      <c r="C8" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="K8" s="3"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12" ht="116" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="C9" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>92</v>
+      </c>
       <c r="K9" s="3"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" ht="116" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+      <c r="C10" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>99</v>
+      </c>
       <c r="K10" s="3"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:12" ht="145" x14ac:dyDescent="0.35">
       <c r="B11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
+      <c r="C11" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>116</v>
+      </c>
       <c r="K11" s="3"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="I12" s="5"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
-        <v>52</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C5201B-6DA7-4669-BEFA-08DD2841F30B}">
+  <dimension ref="B2:L21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="14.36328125" customWidth="1"/>
+    <col min="3" max="3" width="14.90625" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" customWidth="1"/>
+    <col min="5" max="5" width="17.7265625" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" customWidth="1"/>
+    <col min="7" max="7" width="18.1796875" customWidth="1"/>
+    <col min="8" max="8" width="18.54296875" customWidth="1"/>
+    <col min="9" max="9" width="13.81640625" customWidth="1"/>
+    <col min="10" max="10" width="15.81640625" customWidth="1"/>
+    <col min="11" max="11" width="12.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="6"/>
+    </row>
+    <row r="3" spans="2:12" ht="119" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="2:12" ht="116" x14ac:dyDescent="0.35">
+      <c r="B4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="116" x14ac:dyDescent="0.35">
+      <c r="B5" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="116" x14ac:dyDescent="0.35">
+      <c r="B6" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="116" x14ac:dyDescent="0.35">
+      <c r="B7" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="B8" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="B9" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="116" x14ac:dyDescent="0.35">
+      <c r="B10" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B11" s="3"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B12" s="3"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B13" s="3"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B21" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>